<commit_message>
Fixes #2 draft excel back to qualification
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\Qualification-Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFF2D25-78BF-43AF-9BC2-1C1928F66605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CB92CC-BFED-4A20-809D-7F01A787DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16965" windowWidth="29040" windowHeight="15720" tabRatio="814" firstSheet="3" activeTab="14" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="1400" yWindow="1400" windowWidth="14400" windowHeight="7270" tabRatio="814" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Sections" sheetId="11" r:id="rId12"/>
     <sheet name="Inputs" sheetId="12" r:id="rId13"/>
     <sheet name="GlobalPlotSettings" sheetId="13" r:id="rId14"/>
-    <sheet name="GlobalAxes_DDI_PredVsObs" sheetId="14" r:id="rId15"/>
+    <sheet name="GlobalAxesSettings" sheetId="14" r:id="rId15"/>
     <sheet name="Lookup" sheetId="15" r:id="rId16"/>
   </sheets>
   <definedNames>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="173">
   <si>
     <t>ID</t>
   </si>
@@ -578,6 +578,9 @@
   </si>
   <si>
     <t>GridLines</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -1337,35 +1340,39 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4341602-74FC-44F8-95AC-478F4F19D2AA}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1860,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1872,7 +1879,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
2 excel to quali (#19)
* Fixes #2 draft excel back to qualification

* Update test to match ID -> Id

* Fix wrong Id replacements
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\Qualification-Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFF2D25-78BF-43AF-9BC2-1C1928F66605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CB92CC-BFED-4A20-809D-7F01A787DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16965" windowWidth="29040" windowHeight="15720" tabRatio="814" firstSheet="3" activeTab="14" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="1400" yWindow="1400" windowWidth="14400" windowHeight="7270" tabRatio="814" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Sections" sheetId="11" r:id="rId12"/>
     <sheet name="Inputs" sheetId="12" r:id="rId13"/>
     <sheet name="GlobalPlotSettings" sheetId="13" r:id="rId14"/>
-    <sheet name="GlobalAxes_DDI_PredVsObs" sheetId="14" r:id="rId15"/>
+    <sheet name="GlobalAxesSettings" sheetId="14" r:id="rId15"/>
     <sheet name="Lookup" sheetId="15" r:id="rId16"/>
   </sheets>
   <definedNames>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="173">
   <si>
     <t>ID</t>
   </si>
@@ -578,6 +578,9 @@
   </si>
   <si>
     <t>GridLines</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -1337,35 +1340,39 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4341602-74FC-44F8-95AC-478F4F19D2AA}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1860,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1872,7 +1879,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Fixes #24 GOF Merged Plots
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CB92CC-BFED-4A20-809D-7F01A787DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97A363E-88BA-407D-838F-C3C9FCBA6226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1400" windowWidth="14400" windowHeight="7270" tabRatio="814" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="6" activeTab="11" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -20,19 +20,24 @@
     <sheet name="ObsData" sheetId="5" r:id="rId5"/>
     <sheet name="BB" sheetId="2" r:id="rId6"/>
     <sheet name="SimParam" sheetId="3" r:id="rId7"/>
-    <sheet name="CT_Profile" sheetId="8" r:id="rId8"/>
-    <sheet name="CT_Mapping" sheetId="7" r:id="rId9"/>
-    <sheet name="DDI_Ratio" sheetId="9" r:id="rId10"/>
-    <sheet name="DDI_Ratio_Mapping" sheetId="10" r:id="rId11"/>
-    <sheet name="Sections" sheetId="11" r:id="rId12"/>
-    <sheet name="Inputs" sheetId="12" r:id="rId13"/>
-    <sheet name="GlobalPlotSettings" sheetId="13" r:id="rId14"/>
-    <sheet name="GlobalAxesSettings" sheetId="14" r:id="rId15"/>
-    <sheet name="Lookup" sheetId="15" r:id="rId16"/>
+    <sheet name="All_Plots" sheetId="19" r:id="rId8"/>
+    <sheet name="CT_Plots" sheetId="8" r:id="rId9"/>
+    <sheet name="CT_Mapping" sheetId="7" r:id="rId10"/>
+    <sheet name="GOF_Plots" sheetId="17" r:id="rId11"/>
+    <sheet name="GOF_Mapping" sheetId="18" r:id="rId12"/>
+    <sheet name="DDIRatio_Plots" sheetId="9" r:id="rId13"/>
+    <sheet name="DDIRatio_Mapping" sheetId="10" r:id="rId14"/>
+    <sheet name="PKRatio_Plots" sheetId="20" r:id="rId15"/>
+    <sheet name="PKRatio_Mapping" sheetId="21" r:id="rId16"/>
+    <sheet name="Sections" sheetId="11" r:id="rId17"/>
+    <sheet name="Inputs" sheetId="12" r:id="rId18"/>
+    <sheet name="GlobalPlotSettings" sheetId="13" r:id="rId19"/>
+    <sheet name="GlobalAxesSettings" sheetId="14" r:id="rId20"/>
+    <sheet name="Lookup" sheetId="15" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CT_Mapping!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">DDI_Ratio_Mapping!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">CT_Mapping!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">DDIRatio_Mapping!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ObsData!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -56,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="174">
   <si>
     <t>ID</t>
   </si>
@@ -582,12 +587,15 @@
   <si>
     <t>Id</t>
   </si>
+  <si>
+    <t>ObservedDataRecordId</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -613,6 +621,14 @@
     <font>
       <b/>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -645,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -659,6 +675,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,11 +1035,193 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD237D21-BEEB-4E24-9FAD-AAF59B70B9A6}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.453125" customWidth="1"/>
+    <col min="4" max="4" width="46.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3301F9-9944-4A4A-8E79-17917B82ED2F}">
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DC37D1-7554-405A-80D0-6E0B98A7F812}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A769436E-1171-4487-BF5B-BA2851FAA4C1}">
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD25"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1103,57 +1302,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{97866A5A-0A03-4818-A2F9-7F17BD10326C}">
-          <x14:formula1>
-            <xm:f>Lookup!$K$2:$K$34</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EAE83B08-C38B-4033-ACE0-E6C2D40EAF04}">
-          <x14:formula1>
-            <xm:f>Lookup!$N$2:$N$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{51ABA0C2-44C7-40E4-9C48-C4FCFB22A1C9}">
-          <x14:formula1>
-            <xm:f>Lookup!$J$2:$J$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F9EDC60F-229F-4352-9782-131815401A7F}">
-          <x14:formula1>
-            <xm:f>Lookup!$H$2:$H$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{172C6CF1-CC3D-42D9-BFE5-827AFD097564}">
-          <x14:formula1>
-            <xm:f>Lookup!$D$2:$D$22</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F0AB065-98F7-492C-B226-52EBF64079C3}">
-          <x14:formula1>
-            <xm:f>Sections!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432CE1B2-D2E2-4643-B063-1AD97C2500A1}">
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1221,7 +1378,131 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A577CC0-D5A0-4A13-862C-A719AB883B03}">
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5A9D53-FE8C-4361-AB33-ABCEC6AC2D66}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08128445-A22D-4DD1-95E7-BAE3F58A3A3E}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1256,7 +1537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B32FE6-E7C3-432E-AC30-5D65F15848DB}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1291,7 +1572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5BE149-6760-4198-9DB8-B696AF8EFF69}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -1338,7 +1619,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4341602-74FC-44F8-95AC-478F4F19D2AA}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1381,12 +1689,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E983D58-D2D3-4814-B96F-57C00BE3A72F}">
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1856,33 +2164,6 @@
     <row r="34" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K34" s="3" t="s">
         <v>151</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="120.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2096,17 +2377,47 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E643DA-C568-4C07-B83D-DF9A48837ED1}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F83E462-CD2A-4A6E-B117-A1A1EAD04B68}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="A2:Q3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
@@ -2176,83 +2487,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7ED4E49A-3C50-4A96-B45C-2B1DF4EF3107}">
-          <x14:formula1>
-            <xm:f>Lookup!$C$2:$C$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C8D1BD84-A7F7-4723-9FB8-F9B598B4E352}">
-          <x14:formula1>
-            <xm:f>Sections!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD237D21-BEEB-4E24-9FAD-AAF59B70B9A6}">
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.453125" customWidth="1"/>
-    <col min="4" max="4" width="46.81640625" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.36328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixes #24 GOF Merged Plots (#34)
* Fixes #24 GOF Merged Plots

* Fix typo and explain what code does
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CB92CC-BFED-4A20-809D-7F01A787DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97A363E-88BA-407D-838F-C3C9FCBA6226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1400" windowWidth="14400" windowHeight="7270" tabRatio="814" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="6" activeTab="11" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -20,19 +20,24 @@
     <sheet name="ObsData" sheetId="5" r:id="rId5"/>
     <sheet name="BB" sheetId="2" r:id="rId6"/>
     <sheet name="SimParam" sheetId="3" r:id="rId7"/>
-    <sheet name="CT_Profile" sheetId="8" r:id="rId8"/>
-    <sheet name="CT_Mapping" sheetId="7" r:id="rId9"/>
-    <sheet name="DDI_Ratio" sheetId="9" r:id="rId10"/>
-    <sheet name="DDI_Ratio_Mapping" sheetId="10" r:id="rId11"/>
-    <sheet name="Sections" sheetId="11" r:id="rId12"/>
-    <sheet name="Inputs" sheetId="12" r:id="rId13"/>
-    <sheet name="GlobalPlotSettings" sheetId="13" r:id="rId14"/>
-    <sheet name="GlobalAxesSettings" sheetId="14" r:id="rId15"/>
-    <sheet name="Lookup" sheetId="15" r:id="rId16"/>
+    <sheet name="All_Plots" sheetId="19" r:id="rId8"/>
+    <sheet name="CT_Plots" sheetId="8" r:id="rId9"/>
+    <sheet name="CT_Mapping" sheetId="7" r:id="rId10"/>
+    <sheet name="GOF_Plots" sheetId="17" r:id="rId11"/>
+    <sheet name="GOF_Mapping" sheetId="18" r:id="rId12"/>
+    <sheet name="DDIRatio_Plots" sheetId="9" r:id="rId13"/>
+    <sheet name="DDIRatio_Mapping" sheetId="10" r:id="rId14"/>
+    <sheet name="PKRatio_Plots" sheetId="20" r:id="rId15"/>
+    <sheet name="PKRatio_Mapping" sheetId="21" r:id="rId16"/>
+    <sheet name="Sections" sheetId="11" r:id="rId17"/>
+    <sheet name="Inputs" sheetId="12" r:id="rId18"/>
+    <sheet name="GlobalPlotSettings" sheetId="13" r:id="rId19"/>
+    <sheet name="GlobalAxesSettings" sheetId="14" r:id="rId20"/>
+    <sheet name="Lookup" sheetId="15" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CT_Mapping!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">DDI_Ratio_Mapping!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">CT_Mapping!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">DDIRatio_Mapping!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ObsData!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -56,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="174">
   <si>
     <t>ID</t>
   </si>
@@ -582,12 +587,15 @@
   <si>
     <t>Id</t>
   </si>
+  <si>
+    <t>ObservedDataRecordId</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -613,6 +621,14 @@
     <font>
       <b/>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -645,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -659,6 +675,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,11 +1035,193 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD237D21-BEEB-4E24-9FAD-AAF59B70B9A6}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.453125" customWidth="1"/>
+    <col min="4" max="4" width="46.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3301F9-9944-4A4A-8E79-17917B82ED2F}">
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DC37D1-7554-405A-80D0-6E0B98A7F812}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A769436E-1171-4487-BF5B-BA2851FAA4C1}">
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD25"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1103,57 +1302,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{97866A5A-0A03-4818-A2F9-7F17BD10326C}">
-          <x14:formula1>
-            <xm:f>Lookup!$K$2:$K$34</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EAE83B08-C38B-4033-ACE0-E6C2D40EAF04}">
-          <x14:formula1>
-            <xm:f>Lookup!$N$2:$N$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{51ABA0C2-44C7-40E4-9C48-C4FCFB22A1C9}">
-          <x14:formula1>
-            <xm:f>Lookup!$J$2:$J$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F9EDC60F-229F-4352-9782-131815401A7F}">
-          <x14:formula1>
-            <xm:f>Lookup!$H$2:$H$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{172C6CF1-CC3D-42D9-BFE5-827AFD097564}">
-          <x14:formula1>
-            <xm:f>Lookup!$D$2:$D$22</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F0AB065-98F7-492C-B226-52EBF64079C3}">
-          <x14:formula1>
-            <xm:f>Sections!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432CE1B2-D2E2-4643-B063-1AD97C2500A1}">
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1221,7 +1378,131 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A577CC0-D5A0-4A13-862C-A719AB883B03}">
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5A9D53-FE8C-4361-AB33-ABCEC6AC2D66}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08128445-A22D-4DD1-95E7-BAE3F58A3A3E}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1256,7 +1537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B32FE6-E7C3-432E-AC30-5D65F15848DB}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1291,7 +1572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5BE149-6760-4198-9DB8-B696AF8EFF69}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -1338,7 +1619,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4341602-74FC-44F8-95AC-478F4F19D2AA}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1381,12 +1689,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E983D58-D2D3-4814-B96F-57C00BE3A72F}">
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1856,33 +2164,6 @@
     <row r="34" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K34" s="3" t="s">
         <v>151</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="120.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2096,17 +2377,47 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E643DA-C568-4C07-B83D-DF9A48837ED1}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F83E462-CD2A-4A6E-B117-A1A1EAD04B68}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="A2:Q3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
@@ -2176,83 +2487,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7ED4E49A-3C50-4A96-B45C-2B1DF4EF3107}">
-          <x14:formula1>
-            <xm:f>Lookup!$C$2:$C$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C8D1BD84-A7F7-4723-9FB8-F9B598B4E352}">
-          <x14:formula1>
-            <xm:f>Sections!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD237D21-BEEB-4E24-9FAD-AAF59B70B9A6}">
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.453125" customWidth="1"/>
-    <col min="4" max="4" width="46.81640625" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.36328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixes #36 convert inputs and intro
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97A363E-88BA-407D-838F-C3C9FCBA6226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F414920B-844C-4744-B550-77BD027C1817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="6" activeTab="11" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="11" activeTab="17" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -30,10 +30,11 @@
     <sheet name="PKRatio_Plots" sheetId="20" r:id="rId15"/>
     <sheet name="PKRatio_Mapping" sheetId="21" r:id="rId16"/>
     <sheet name="Sections" sheetId="11" r:id="rId17"/>
-    <sheet name="Inputs" sheetId="12" r:id="rId18"/>
-    <sheet name="GlobalPlotSettings" sheetId="13" r:id="rId19"/>
-    <sheet name="GlobalAxesSettings" sheetId="14" r:id="rId20"/>
-    <sheet name="Lookup" sheetId="15" r:id="rId21"/>
+    <sheet name="Intro" sheetId="22" r:id="rId18"/>
+    <sheet name="Inputs" sheetId="12" r:id="rId19"/>
+    <sheet name="GlobalPlotSettings" sheetId="13" r:id="rId20"/>
+    <sheet name="GlobalAxesSettings" sheetId="14" r:id="rId21"/>
+    <sheet name="Lookup" sheetId="15" r:id="rId22"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">CT_Mapping!$A$1:$J$1</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="174">
   <si>
     <t>ID</t>
   </si>
@@ -1177,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DC37D1-7554-405A-80D0-6E0B98A7F812}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
@@ -1506,9 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08128445-A22D-4DD1-95E7-BAE3F58A3A3E}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1538,6 +1537,26 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9520BD4-3B1E-4ED1-BC10-62695299EC6C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B32FE6-E7C3-432E-AC30-5D65F15848DB}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1572,7 +1591,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5BE149-6760-4198-9DB8-B696AF8EFF69}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -1619,34 +1665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="120.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4341602-74FC-44F8-95AC-478F4F19D2AA}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1689,7 +1708,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E983D58-D2D3-4814-B96F-57C00BE3A72F}">
   <dimension ref="A1:P34"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fixes #36 convert inputs and intro (#39)
* Fixes #36 convert inputs and intro

* Update R/excel-qualification.R

Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>

* Update R/excel-qualification.R

Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>

* Explicit return in lapply

---------

Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97A363E-88BA-407D-838F-C3C9FCBA6226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F414920B-844C-4744-B550-77BD027C1817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="6" activeTab="11" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="11" activeTab="17" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -30,10 +30,11 @@
     <sheet name="PKRatio_Plots" sheetId="20" r:id="rId15"/>
     <sheet name="PKRatio_Mapping" sheetId="21" r:id="rId16"/>
     <sheet name="Sections" sheetId="11" r:id="rId17"/>
-    <sheet name="Inputs" sheetId="12" r:id="rId18"/>
-    <sheet name="GlobalPlotSettings" sheetId="13" r:id="rId19"/>
-    <sheet name="GlobalAxesSettings" sheetId="14" r:id="rId20"/>
-    <sheet name="Lookup" sheetId="15" r:id="rId21"/>
+    <sheet name="Intro" sheetId="22" r:id="rId18"/>
+    <sheet name="Inputs" sheetId="12" r:id="rId19"/>
+    <sheet name="GlobalPlotSettings" sheetId="13" r:id="rId20"/>
+    <sheet name="GlobalAxesSettings" sheetId="14" r:id="rId21"/>
+    <sheet name="Lookup" sheetId="15" r:id="rId22"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">CT_Mapping!$A$1:$J$1</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="174">
   <si>
     <t>ID</t>
   </si>
@@ -1177,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DC37D1-7554-405A-80D0-6E0B98A7F812}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
@@ -1506,9 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08128445-A22D-4DD1-95E7-BAE3F58A3A3E}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1538,6 +1537,26 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9520BD4-3B1E-4ED1-BC10-62695299EC6C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B32FE6-E7C3-432E-AC30-5D65F15848DB}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1572,7 +1591,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5BE149-6760-4198-9DB8-B696AF8EFF69}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -1619,34 +1665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="120.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4341602-74FC-44F8-95AC-478F4F19D2AA}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1689,7 +1708,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E983D58-D2D3-4814-B96F-57C00BE3A72F}">
   <dimension ref="A1:P34"/>
   <sheetViews>

</xml_diff>

<commit_message>
Use centralized Excel Template for defining global variables
The new excel template actually Fixes #33 as the lookup table now includes the default colors and rules to match the fill color when selecting colors from the list
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F414920B-844C-4744-B550-77BD027C1817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF554AD-D822-48DE-9915-30EA1CA5B30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="11" activeTab="17" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="5370" yWindow="-12120" windowWidth="19440" windowHeight="11520" tabRatio="814" firstSheet="1" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Dimensionless</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>Log</t>
   </si>
   <si>
@@ -388,12 +385,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Concentration(mass)</t>
-  </si>
-  <si>
-    <t>Concentration(molar)</t>
-  </si>
-  <si>
     <t>Fraction</t>
   </si>
   <si>
@@ -539,9 +530,6 @@
   </si>
   <si>
     <t>Boolean</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>Simulation_Control</t>
@@ -590,13 +578,70 @@
   </si>
   <si>
     <t>ObservedDataRecordId</t>
+  </si>
+  <si>
+    <t>AxesSettingsPlots</t>
+  </si>
+  <si>
+    <t>GOFMergedPlotsPredictedVsObserved</t>
+  </si>
+  <si>
+    <t>GOFMergedPlotsResidualsOverTime</t>
+  </si>
+  <si>
+    <t>DDIRatioPlotsPredictedVsObserved</t>
+  </si>
+  <si>
+    <t>DDIRatioPlotsResidualsVsObserved</t>
+  </si>
+  <si>
+    <t>ComparisonTimeProfile</t>
+  </si>
+  <si>
+    <t>PKRatioPlots</t>
+  </si>
+  <si>
+    <t>#CC6677</t>
+  </si>
+  <si>
+    <t>#332288</t>
+  </si>
+  <si>
+    <t>#DDCC77</t>
+  </si>
+  <si>
+    <t>#117733</t>
+  </si>
+  <si>
+    <t>#88CCEE</t>
+  </si>
+  <si>
+    <t>#882255</t>
+  </si>
+  <si>
+    <t>#44AA99</t>
+  </si>
+  <si>
+    <t>#999933</t>
+  </si>
+  <si>
+    <t>#AA4499</t>
+  </si>
+  <si>
+    <t>#DDDDDD</t>
+  </si>
+  <si>
+    <t>Concentration (mass)</t>
+  </si>
+  <si>
+    <t>Concentration (molar)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,8 +680,78 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCC6677"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF332288"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFDDCC77"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF117733"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF88CCEE"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF882255"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF44AA99"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF999933"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFAA4499"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFDDDDDD"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,6 +761,72 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC6677"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF332288"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDCC77"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF117733"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF88CCEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF882255"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF44AA99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999933"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAA4499"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,27 +843,458 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color rgb="FFCC6677"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC6677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF332288"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF332288"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDCC77"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDDCC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF117733"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF117733"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF88CCEE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF88CCEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF882255"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF882255"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF44AA99"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF44AA99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF999933"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAA4499"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA4499"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDDDDD"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC6677"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC6677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF332288"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF332288"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDCC77"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDDCC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF117733"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF117733"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF88CCEE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF88CCEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF882255"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF882255"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF44AA99"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF44AA99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF999933"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAA4499"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA4499"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDDDDD"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC6677"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC6677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF332288"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF332288"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDCC77"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDDCC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF117733"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF117733"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF88CCEE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF88CCEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF882255"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF882255"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF44AA99"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF44AA99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF999933"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAA4499"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA4499"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDDDDD"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC6677"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC6677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF332288"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF332288"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDCC77"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDDCC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF117733"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF117733"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF88CCEE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF88CCEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF882255"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF882255"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF44AA99"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF44AA99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF999933"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAA4499"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA4499"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDDDDD"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDDDDDD"/>
+      <color rgb="FFAA4499"/>
+      <color rgb="FF999933"/>
+      <color rgb="FF44AA99"/>
+      <color rgb="FF882255"/>
+      <color rgb="FF88CCEE"/>
+      <color rgb="FF117733"/>
+      <color rgb="FFDDCC77"/>
+      <color rgb="FF332288"/>
+      <color rgb="FFCC6677"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1013,7 +1625,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EDCB13-CEE1-4630-80E7-2767E804FDDB}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1022,12 +1636,12 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>169</v>
+      <c r="A2" s="7" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1039,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD237D21-BEEB-4E24-9FAD-AAF59B70B9A6}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD18"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1091,6 +1705,157 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{743E33FB-D43E-4375-9FCF-25F663B4940E}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,H2)))</xm:f>
+            <xm:f>Lookup!$E$11</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDDDDD"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFDDDDDD"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{C535E228-289D-45D9-9282-879CE6E2C64E}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,H2)))</xm:f>
+            <xm:f>Lookup!$E$10</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFAA4499"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFAA4499"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{95835526-B51F-4B16-97D0-020CF6328F71}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,H2)))</xm:f>
+            <xm:f>Lookup!$E$9</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF999933"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF999933"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{5C23FC05-D515-47CD-AF59-F37016F19397}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,H2)))</xm:f>
+            <xm:f>Lookup!$E$8</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF44AA99"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF44AA99"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{72B42695-5629-44A0-8809-8999D86A5EAA}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,H2)))</xm:f>
+            <xm:f>Lookup!$E$7</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF882255"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF882255"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{ABA67EE8-FD7A-434F-B572-1E401062FABB}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,H2)))</xm:f>
+            <xm:f>Lookup!$E$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF88CCEE"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF88CCEE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{4E2105A6-5FAA-4A18-8E98-AF36CC254DD6}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,H2)))</xm:f>
+            <xm:f>Lookup!$E$5</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF117733"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF117733"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{66A1085C-AD9E-4CCF-9A02-21201B9A96D5}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,H2)))</xm:f>
+            <xm:f>Lookup!$E$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDCC77"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor auto="1"/>
+                  <bgColor rgb="FFDDCC77"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{D83B7393-2B82-4CC4-BA70-68E042994C09}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,H2)))</xm:f>
+            <xm:f>Lookup!$E$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF332288"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF332288"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{C9CE015A-E457-49C5-97CD-F5A5A6CAAAB5}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,H2)))</xm:f>
+            <xm:f>Lookup!$E$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFCC6677"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCC6677"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H2:H100</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1111,62 +1876,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1179,7 +1944,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="G2" sqref="G2:G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1214,6 +1979,156 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{E0011040-6304-4C2D-881E-45C7F3CE34BD}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,G2)))</xm:f>
+            <xm:f>Lookup!$E$11</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDDDDD"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFDDDDDD"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{BC9D4CF0-84A4-4C50-9D7A-E58CFB923F1E}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,G2)))</xm:f>
+            <xm:f>Lookup!$E$10</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFAA4499"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFAA4499"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{BB3CBDB4-5B6B-41AC-B3D2-9AE4E87ED5BB}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,G2)))</xm:f>
+            <xm:f>Lookup!$E$9</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF999933"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF999933"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{784924CF-29F0-46EC-BB3D-238D671A8525}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,G2)))</xm:f>
+            <xm:f>Lookup!$E$8</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF44AA99"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF44AA99"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{D523D052-97F1-4BEF-893E-733B95C31110}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,G2)))</xm:f>
+            <xm:f>Lookup!$E$7</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF882255"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF882255"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{7FEE5258-924B-4F1B-BD78-7A6E99F382FE}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,G2)))</xm:f>
+            <xm:f>Lookup!$E$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF88CCEE"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF88CCEE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{FFF65803-65BA-40EC-A715-986B17D506EE}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,G2)))</xm:f>
+            <xm:f>Lookup!$E$5</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF117733"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF117733"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{A9E1A033-026E-4891-8E06-FABE8F6A8201}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,G2)))</xm:f>
+            <xm:f>Lookup!$E$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDCC77"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor auto="1"/>
+                  <bgColor rgb="FFDDCC77"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{B669755B-ECFB-4A14-9A6D-F4381D2B9003}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,G2)))</xm:f>
+            <xm:f>Lookup!$E$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF332288"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF332288"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{162C8744-83A7-4F7B-AEEA-1932220E8980}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,G2)))</xm:f>
+            <xm:f>Lookup!$E$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFCC6677"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCC6677"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G2:G100</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1222,7 +2137,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H2" sqref="H2:H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1283,26 +2198,176 @@
         <v>54</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{51027A57-3EFE-4C18-8F44-2F04B93E96DD}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,H2)))</xm:f>
+            <xm:f>Lookup!$E$11</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDDDDD"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFDDDDDD"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{BA0AEECD-11CA-4006-A873-213B33E32ABC}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,H2)))</xm:f>
+            <xm:f>Lookup!$E$10</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFAA4499"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFAA4499"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{02182748-E97B-4067-BC6E-59258DEE0183}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,H2)))</xm:f>
+            <xm:f>Lookup!$E$9</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF999933"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF999933"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{2D34B9F3-462F-4ADE-83B8-F75B527DE26B}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,H2)))</xm:f>
+            <xm:f>Lookup!$E$8</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF44AA99"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF44AA99"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{1BC06D6C-F534-466C-8003-E270BB9C9D0E}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,H2)))</xm:f>
+            <xm:f>Lookup!$E$7</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF882255"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF882255"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{12914CFE-3875-4549-8307-C052C9C7970D}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,H2)))</xm:f>
+            <xm:f>Lookup!$E$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF88CCEE"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF88CCEE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{F35E664A-B150-4A3C-A008-053EFC62F36A}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,H2)))</xm:f>
+            <xm:f>Lookup!$E$5</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF117733"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF117733"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{36E5034E-AEB7-4BCE-869D-52E98AA7AC73}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,H2)))</xm:f>
+            <xm:f>Lookup!$E$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDCC77"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor auto="1"/>
+                  <bgColor rgb="FFDDCC77"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{885BE7A6-31A7-4BE3-AE17-08048EED1D00}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,H2)))</xm:f>
+            <xm:f>Lookup!$E$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF332288"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF332288"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{4B57DE8B-BE93-4EB0-AB4D-E4D41D82FF58}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,H2)))</xm:f>
+            <xm:f>Lookup!$E$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFCC6677"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCC6677"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H2:H100</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1331,46 +2396,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="F1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1384,7 +2449,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E2" sqref="E2:E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1438,26 +2503,176 @@
         <v>54</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{122FD37C-2CD4-424F-8509-5E2E9FEA8569}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,E2)))</xm:f>
+            <xm:f>Lookup!$E$11</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDDDDD"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFDDDDDD"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{62C66900-2092-418B-8DC2-8592CA91653C}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,E2)))</xm:f>
+            <xm:f>Lookup!$E$10</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFAA4499"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFAA4499"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{E9D8C9E9-05BA-469B-8EB2-3B77645E7749}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,E2)))</xm:f>
+            <xm:f>Lookup!$E$9</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF999933"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF999933"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{BBD1427C-3DB1-48B0-BCD3-CE8B144AC0AD}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,E2)))</xm:f>
+            <xm:f>Lookup!$E$8</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF44AA99"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF44AA99"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{C160719F-A188-4FE0-9C8C-74252EE20D95}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,E2)))</xm:f>
+            <xm:f>Lookup!$E$7</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF882255"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF882255"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{4A569E89-E3F0-42BA-95D8-4F9551719D1A}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,E2)))</xm:f>
+            <xm:f>Lookup!$E$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF88CCEE"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF88CCEE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{8A00930E-F479-478A-8D4B-7E6C8B256E49}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,E2)))</xm:f>
+            <xm:f>Lookup!$E$5</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF117733"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF117733"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{FD135833-5C75-4341-BD84-3B2F4162410A}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,E2)))</xm:f>
+            <xm:f>Lookup!$E$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDCC77"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor auto="1"/>
+                  <bgColor rgb="FFDDCC77"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{A1E405FC-112F-4528-AA72-9DDD2F5A96B4}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,E2)))</xm:f>
+            <xm:f>Lookup!$E$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF332288"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF332288"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{10D4F4A8-549E-4809-94C0-FA303CB7E0A6}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,E2)))</xm:f>
+            <xm:f>Lookup!$E$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFCC6677"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCC6677"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E2:E100</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1489,7 +2704,7 @@
         <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>20</v>
@@ -1540,7 +2755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9520BD4-3B1E-4ED1-BC10-62695299EC6C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -1595,9 +2810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1607,7 +2820,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1669,9 +2882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4341602-74FC-44F8-95AC-478F4F19D2AA}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1694,10 +2905,10 @@
         <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>57</v>
@@ -1710,10 +2921,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E983D58-D2D3-4814-B96F-57C00BE3A72F}">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1722,468 +2933,989 @@
     <col min="2" max="2" width="23.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="E4" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M4" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="3" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K7" s="3" t="s">
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="K8" s="3" t="s">
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K9" s="3" t="s">
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="K10" s="3" t="s">
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D11" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K11" s="3" t="s">
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D12" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="K12" s="3" t="s">
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D13" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="3" t="s">
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K14" s="3" t="s">
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D15" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="K15" s="3" t="s">
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D16" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K16" s="3" t="s">
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D17" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="K17" s="3" t="s">
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D18" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="K18" s="3" t="s">
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D19" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K19" s="3" t="s">
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D20" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K20" s="3" t="s">
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D21" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="K21" s="3" t="s">
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D22" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K22" s="3" t="s">
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K23" s="3" t="s">
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K24" s="3" t="s">
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K25" s="3" t="s">
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K26" s="3" t="s">
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K27" s="3" t="s">
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K28" s="3" t="s">
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K29" s="3" t="s">
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K30" s="3" t="s">
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K31" s="3" t="s">
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K32" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K33" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K34" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2351,16 +4083,16 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2486,22 +4218,22 @@
         <v>54</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
32 data validation (#54)
* Use centralized Excel Template for defining global variables

The new excel template actually Fixes #33 as the lookup table now includes the default colors and rules to match the fill color when selecting colors from the list

* Fixes #32 introduction of dataValidation wrapper

* Apply changes suggested by copliot
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F414920B-844C-4744-B550-77BD027C1817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF554AD-D822-48DE-9915-30EA1CA5B30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="11" activeTab="17" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="5370" yWindow="-12120" windowWidth="19440" windowHeight="11520" tabRatio="814" firstSheet="1" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Dimensionless</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>Log</t>
   </si>
   <si>
@@ -388,12 +385,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Concentration(mass)</t>
-  </si>
-  <si>
-    <t>Concentration(molar)</t>
-  </si>
-  <si>
     <t>Fraction</t>
   </si>
   <si>
@@ -539,9 +530,6 @@
   </si>
   <si>
     <t>Boolean</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>Simulation_Control</t>
@@ -590,13 +578,70 @@
   </si>
   <si>
     <t>ObservedDataRecordId</t>
+  </si>
+  <si>
+    <t>AxesSettingsPlots</t>
+  </si>
+  <si>
+    <t>GOFMergedPlotsPredictedVsObserved</t>
+  </si>
+  <si>
+    <t>GOFMergedPlotsResidualsOverTime</t>
+  </si>
+  <si>
+    <t>DDIRatioPlotsPredictedVsObserved</t>
+  </si>
+  <si>
+    <t>DDIRatioPlotsResidualsVsObserved</t>
+  </si>
+  <si>
+    <t>ComparisonTimeProfile</t>
+  </si>
+  <si>
+    <t>PKRatioPlots</t>
+  </si>
+  <si>
+    <t>#CC6677</t>
+  </si>
+  <si>
+    <t>#332288</t>
+  </si>
+  <si>
+    <t>#DDCC77</t>
+  </si>
+  <si>
+    <t>#117733</t>
+  </si>
+  <si>
+    <t>#88CCEE</t>
+  </si>
+  <si>
+    <t>#882255</t>
+  </si>
+  <si>
+    <t>#44AA99</t>
+  </si>
+  <si>
+    <t>#999933</t>
+  </si>
+  <si>
+    <t>#AA4499</t>
+  </si>
+  <si>
+    <t>#DDDDDD</t>
+  </si>
+  <si>
+    <t>Concentration (mass)</t>
+  </si>
+  <si>
+    <t>Concentration (molar)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,8 +680,78 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCC6677"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF332288"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFDDCC77"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF117733"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF88CCEE"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF882255"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF44AA99"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF999933"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFAA4499"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFDDDDDD"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,6 +761,72 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC6677"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF332288"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDCC77"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF117733"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF88CCEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF882255"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF44AA99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999933"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAA4499"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,27 +843,458 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color rgb="FFCC6677"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC6677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF332288"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF332288"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDCC77"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDDCC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF117733"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF117733"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF88CCEE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF88CCEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF882255"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF882255"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF44AA99"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF44AA99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF999933"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAA4499"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA4499"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDDDDD"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC6677"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC6677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF332288"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF332288"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDCC77"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDDCC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF117733"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF117733"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF88CCEE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF88CCEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF882255"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF882255"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF44AA99"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF44AA99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF999933"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAA4499"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA4499"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDDDDD"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC6677"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC6677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF332288"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF332288"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDCC77"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDDCC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF117733"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF117733"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF88CCEE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF88CCEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF882255"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF882255"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF44AA99"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF44AA99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF999933"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAA4499"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA4499"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDDDDD"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC6677"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC6677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF332288"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF332288"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDCC77"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDDCC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF117733"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF117733"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF88CCEE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF88CCEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF882255"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF882255"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF44AA99"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF44AA99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF999933"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAA4499"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA4499"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDDDDD"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDDDDDD"/>
+      <color rgb="FFAA4499"/>
+      <color rgb="FF999933"/>
+      <color rgb="FF44AA99"/>
+      <color rgb="FF882255"/>
+      <color rgb="FF88CCEE"/>
+      <color rgb="FF117733"/>
+      <color rgb="FFDDCC77"/>
+      <color rgb="FF332288"/>
+      <color rgb="FFCC6677"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1013,7 +1625,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EDCB13-CEE1-4630-80E7-2767E804FDDB}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1022,12 +1636,12 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>169</v>
+      <c r="A2" s="7" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1039,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD237D21-BEEB-4E24-9FAD-AAF59B70B9A6}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD18"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1091,6 +1705,157 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{743E33FB-D43E-4375-9FCF-25F663B4940E}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,H2)))</xm:f>
+            <xm:f>Lookup!$E$11</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDDDDD"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFDDDDDD"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{C535E228-289D-45D9-9282-879CE6E2C64E}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,H2)))</xm:f>
+            <xm:f>Lookup!$E$10</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFAA4499"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFAA4499"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{95835526-B51F-4B16-97D0-020CF6328F71}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,H2)))</xm:f>
+            <xm:f>Lookup!$E$9</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF999933"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF999933"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{5C23FC05-D515-47CD-AF59-F37016F19397}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,H2)))</xm:f>
+            <xm:f>Lookup!$E$8</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF44AA99"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF44AA99"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{72B42695-5629-44A0-8809-8999D86A5EAA}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,H2)))</xm:f>
+            <xm:f>Lookup!$E$7</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF882255"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF882255"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{ABA67EE8-FD7A-434F-B572-1E401062FABB}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,H2)))</xm:f>
+            <xm:f>Lookup!$E$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF88CCEE"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF88CCEE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{4E2105A6-5FAA-4A18-8E98-AF36CC254DD6}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,H2)))</xm:f>
+            <xm:f>Lookup!$E$5</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF117733"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF117733"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{66A1085C-AD9E-4CCF-9A02-21201B9A96D5}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,H2)))</xm:f>
+            <xm:f>Lookup!$E$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDCC77"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor auto="1"/>
+                  <bgColor rgb="FFDDCC77"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{D83B7393-2B82-4CC4-BA70-68E042994C09}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,H2)))</xm:f>
+            <xm:f>Lookup!$E$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF332288"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF332288"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{C9CE015A-E457-49C5-97CD-F5A5A6CAAAB5}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,H2)))</xm:f>
+            <xm:f>Lookup!$E$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFCC6677"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCC6677"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H2:H100</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1111,62 +1876,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1179,7 +1944,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="G2" sqref="G2:G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1214,6 +1979,156 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{E0011040-6304-4C2D-881E-45C7F3CE34BD}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,G2)))</xm:f>
+            <xm:f>Lookup!$E$11</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDDDDD"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFDDDDDD"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{BC9D4CF0-84A4-4C50-9D7A-E58CFB923F1E}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,G2)))</xm:f>
+            <xm:f>Lookup!$E$10</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFAA4499"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFAA4499"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{BB3CBDB4-5B6B-41AC-B3D2-9AE4E87ED5BB}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,G2)))</xm:f>
+            <xm:f>Lookup!$E$9</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF999933"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF999933"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{784924CF-29F0-46EC-BB3D-238D671A8525}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,G2)))</xm:f>
+            <xm:f>Lookup!$E$8</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF44AA99"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF44AA99"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{D523D052-97F1-4BEF-893E-733B95C31110}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,G2)))</xm:f>
+            <xm:f>Lookup!$E$7</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF882255"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF882255"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{7FEE5258-924B-4F1B-BD78-7A6E99F382FE}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,G2)))</xm:f>
+            <xm:f>Lookup!$E$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF88CCEE"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF88CCEE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{FFF65803-65BA-40EC-A715-986B17D506EE}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,G2)))</xm:f>
+            <xm:f>Lookup!$E$5</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF117733"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF117733"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{A9E1A033-026E-4891-8E06-FABE8F6A8201}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,G2)))</xm:f>
+            <xm:f>Lookup!$E$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDCC77"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor auto="1"/>
+                  <bgColor rgb="FFDDCC77"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{B669755B-ECFB-4A14-9A6D-F4381D2B9003}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,G2)))</xm:f>
+            <xm:f>Lookup!$E$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF332288"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF332288"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{162C8744-83A7-4F7B-AEEA-1932220E8980}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,G2)))</xm:f>
+            <xm:f>Lookup!$E$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFCC6677"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCC6677"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G2:G100</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1222,7 +2137,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H2" sqref="H2:H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1283,26 +2198,176 @@
         <v>54</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{51027A57-3EFE-4C18-8F44-2F04B93E96DD}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,H2)))</xm:f>
+            <xm:f>Lookup!$E$11</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDDDDD"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFDDDDDD"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{BA0AEECD-11CA-4006-A873-213B33E32ABC}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,H2)))</xm:f>
+            <xm:f>Lookup!$E$10</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFAA4499"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFAA4499"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{02182748-E97B-4067-BC6E-59258DEE0183}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,H2)))</xm:f>
+            <xm:f>Lookup!$E$9</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF999933"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF999933"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{2D34B9F3-462F-4ADE-83B8-F75B527DE26B}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,H2)))</xm:f>
+            <xm:f>Lookup!$E$8</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF44AA99"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF44AA99"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{1BC06D6C-F534-466C-8003-E270BB9C9D0E}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,H2)))</xm:f>
+            <xm:f>Lookup!$E$7</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF882255"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF882255"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{12914CFE-3875-4549-8307-C052C9C7970D}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,H2)))</xm:f>
+            <xm:f>Lookup!$E$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF88CCEE"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF88CCEE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{F35E664A-B150-4A3C-A008-053EFC62F36A}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,H2)))</xm:f>
+            <xm:f>Lookup!$E$5</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF117733"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF117733"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{36E5034E-AEB7-4BCE-869D-52E98AA7AC73}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,H2)))</xm:f>
+            <xm:f>Lookup!$E$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDCC77"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor auto="1"/>
+                  <bgColor rgb="FFDDCC77"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{885BE7A6-31A7-4BE3-AE17-08048EED1D00}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,H2)))</xm:f>
+            <xm:f>Lookup!$E$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF332288"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF332288"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{4B57DE8B-BE93-4EB0-AB4D-E4D41D82FF58}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,H2)))</xm:f>
+            <xm:f>Lookup!$E$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFCC6677"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCC6677"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H2:H100</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1331,46 +2396,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="F1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1384,7 +2449,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E2" sqref="E2:E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1438,26 +2503,176 @@
         <v>54</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{122FD37C-2CD4-424F-8509-5E2E9FEA8569}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,E2)))</xm:f>
+            <xm:f>Lookup!$E$11</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDDDDD"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFDDDDDD"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{62C66900-2092-418B-8DC2-8592CA91653C}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,E2)))</xm:f>
+            <xm:f>Lookup!$E$10</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFAA4499"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFAA4499"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{E9D8C9E9-05BA-469B-8EB2-3B77645E7749}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,E2)))</xm:f>
+            <xm:f>Lookup!$E$9</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF999933"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF999933"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{BBD1427C-3DB1-48B0-BCD3-CE8B144AC0AD}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,E2)))</xm:f>
+            <xm:f>Lookup!$E$8</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF44AA99"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF44AA99"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{C160719F-A188-4FE0-9C8C-74252EE20D95}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,E2)))</xm:f>
+            <xm:f>Lookup!$E$7</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF882255"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF882255"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{4A569E89-E3F0-42BA-95D8-4F9551719D1A}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,E2)))</xm:f>
+            <xm:f>Lookup!$E$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF88CCEE"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF88CCEE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{8A00930E-F479-478A-8D4B-7E6C8B256E49}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,E2)))</xm:f>
+            <xm:f>Lookup!$E$5</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF117733"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF117733"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{FD135833-5C75-4341-BD84-3B2F4162410A}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,E2)))</xm:f>
+            <xm:f>Lookup!$E$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFDDCC77"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor auto="1"/>
+                  <bgColor rgb="FFDDCC77"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{A1E405FC-112F-4528-AA72-9DDD2F5A96B4}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,E2)))</xm:f>
+            <xm:f>Lookup!$E$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF332288"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF332288"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{10D4F4A8-549E-4809-94C0-FA303CB7E0A6}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,E2)))</xm:f>
+            <xm:f>Lookup!$E$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFCC6677"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCC6677"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E2:E100</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1489,7 +2704,7 @@
         <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>20</v>
@@ -1540,7 +2755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9520BD4-3B1E-4ED1-BC10-62695299EC6C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -1595,9 +2810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1607,7 +2820,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1669,9 +2882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4341602-74FC-44F8-95AC-478F4F19D2AA}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1694,10 +2905,10 @@
         <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>57</v>
@@ -1710,10 +2921,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E983D58-D2D3-4814-B96F-57C00BE3A72F}">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1722,468 +2933,989 @@
     <col min="2" max="2" width="23.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="E4" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M4" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="3" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K7" s="3" t="s">
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="K8" s="3" t="s">
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K9" s="3" t="s">
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="K10" s="3" t="s">
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D11" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K11" s="3" t="s">
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D12" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="K12" s="3" t="s">
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D13" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="3" t="s">
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K14" s="3" t="s">
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D15" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="K15" s="3" t="s">
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D16" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K16" s="3" t="s">
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D17" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="K17" s="3" t="s">
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D18" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="K18" s="3" t="s">
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D19" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K19" s="3" t="s">
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D20" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K20" s="3" t="s">
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D21" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="K21" s="3" t="s">
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D22" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K22" s="3" t="s">
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K23" s="3" t="s">
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K24" s="3" t="s">
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K25" s="3" t="s">
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K26" s="3" t="s">
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K27" s="3" t="s">
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K28" s="3" t="s">
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K29" s="3" t="s">
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K30" s="3" t="s">
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K31" s="3" t="s">
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="K32" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K33" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K34" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2351,16 +4083,16 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2486,22 +4218,22 @@
         <v>54</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes #52 include Simulation Paramters in conversion
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF554AD-D822-48DE-9915-30EA1CA5B30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ACCB5F-0663-4CE0-B0B6-2E8E25C37A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="-12120" windowWidth="19440" windowHeight="11520" tabRatio="814" firstSheet="1" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="1" activeTab="6" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -843,11 +843,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1640,7 +1639,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1876,61 +1875,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2395,47 +2394,47 @@
     <col min="14" max="14" width="18.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2810,7 +2809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2946,976 +2945,976 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="10" t="b">
+      <c r="Q2" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="9" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10" t="b">
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10" t="s">
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10" t="s">
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10" t="s">
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10" t="s">
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10" t="s">
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10" t="s">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10" t="s">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10" t="s">
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10" t="s">
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10" t="s">
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="10"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4063,10 +4062,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC45D43-7DB0-4999-A671-8DD063ABA038}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4095,35 +4094,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{028D4E78-A0C9-45BC-89AE-7624549C5BF7}">
-          <x14:formula1>
-            <xm:f>Projects!$A$2:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77DBAA37-CCFD-4C86-BC83-1518AFA04525}">
-          <x14:formula1>
-            <xm:f>Simulations_Outputs!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F31F7B7B-4A8B-4A27-9428-25F7024651B9}">
-          <x14:formula1>
-            <xm:f>Simulations_Outputs!$B$2:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixes #52 include Simulation Paramters in conversion (#55)
* Fixes #52 include Simulation Paramters in conversion

* Remove unnecessary line of code

* Apply suggestions from code review

Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>

---------

Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF554AD-D822-48DE-9915-30EA1CA5B30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ACCB5F-0663-4CE0-B0B6-2E8E25C37A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="-12120" windowWidth="19440" windowHeight="11520" tabRatio="814" firstSheet="1" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="1" activeTab="6" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -843,11 +843,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1640,7 +1639,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1876,61 +1875,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2395,47 +2394,47 @@
     <col min="14" max="14" width="18.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2810,7 +2809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2946,976 +2945,976 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="10" t="b">
+      <c r="Q2" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="9" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10" t="b">
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10" t="s">
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10" t="s">
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10" t="s">
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10" t="s">
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10" t="s">
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10" t="s">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10" t="s">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10" t="s">
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10" t="s">
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10" t="s">
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="10"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4063,10 +4062,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC45D43-7DB0-4999-A671-8DD063ABA038}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4095,35 +4094,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{028D4E78-A0C9-45BC-89AE-7624549C5BF7}">
-          <x14:formula1>
-            <xm:f>Projects!$A$2:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77DBAA37-CCFD-4C86-BC83-1518AFA04525}">
-          <x14:formula1>
-            <xm:f>Simulations_Outputs!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F31F7B7B-4A8B-4A27-9428-25F7024651B9}">
-          <x14:formula1>
-            <xm:f>Simulations_Outputs!$B$2:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update template showing PK Ratio colors
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ACCB5F-0663-4CE0-B0B6-2E8E25C37A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0C9AF4-8E40-421B-9A36-129761BFCC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="1" activeTab="6" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="7" activeTab="14" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -873,7 +873,108 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="50">
+    <dxf>
+      <font>
+        <color rgb="FFCC6677"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC6677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF332288"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF332288"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDCC77"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDDCC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF117733"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF117733"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF88CCEE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF88CCEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF882255"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF882255"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF44AA99"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF44AA99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF999933"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAA4499"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA4499"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDDDDD"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFCC6677"/>
@@ -2135,7 +2236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A769436E-1171-4487-BF5B-BA2851FAA4C1}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H100"/>
     </sheetView>
   </sheetViews>
@@ -2445,10 +2546,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A577CC0-D5A0-4A13-862C-A719AB883B03}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2456,12 +2557,13 @@
     <col min="1" max="1" width="25.81640625" customWidth="1"/>
     <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -2472,51 +2574,54 @@
         <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2526,8 +2631,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{122FD37C-2CD4-424F-8509-5E2E9FEA8569}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{4628622E-2F63-4491-A459-DB1F046D862C}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,F2)))</xm:f>
             <xm:f>Lookup!$E$11</xm:f>
             <x14:dxf>
               <font>
@@ -2540,8 +2645,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{62C66900-2092-418B-8DC2-8592CA91653C}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{E4A88C5B-61F3-48DF-9161-9DC4AD222169}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,F2)))</xm:f>
             <xm:f>Lookup!$E$10</xm:f>
             <x14:dxf>
               <font>
@@ -2554,8 +2659,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{E9D8C9E9-05BA-469B-8EB2-3B77645E7749}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{C753A7B6-EE29-4502-A4B3-4DB24EA9C6FA}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,F2)))</xm:f>
             <xm:f>Lookup!$E$9</xm:f>
             <x14:dxf>
               <font>
@@ -2568,8 +2673,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{BBD1427C-3DB1-48B0-BCD3-CE8B144AC0AD}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{A7363563-7105-4ED0-B895-D72413AB1510}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,F2)))</xm:f>
             <xm:f>Lookup!$E$8</xm:f>
             <x14:dxf>
               <font>
@@ -2582,8 +2687,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{C160719F-A188-4FE0-9C8C-74252EE20D95}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{20D19E1E-214A-4D14-BDB1-54F287803AD0}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,F2)))</xm:f>
             <xm:f>Lookup!$E$7</xm:f>
             <x14:dxf>
               <font>
@@ -2596,8 +2701,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{4A569E89-E3F0-42BA-95D8-4F9551719D1A}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{F4DC78DB-B917-4FE1-B2EC-5D205A6C99BB}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,F2)))</xm:f>
             <xm:f>Lookup!$E$6</xm:f>
             <x14:dxf>
               <font>
@@ -2610,8 +2715,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{8A00930E-F479-478A-8D4B-7E6C8B256E49}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{31946866-D629-4B7B-B3BA-E63CD387DA23}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,F2)))</xm:f>
             <xm:f>Lookup!$E$5</xm:f>
             <x14:dxf>
               <font>
@@ -2624,8 +2729,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{FD135833-5C75-4341-BD84-3B2F4162410A}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{DBEECD34-0320-470A-B068-24CFF47FC76E}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,F2)))</xm:f>
             <xm:f>Lookup!$E$4</xm:f>
             <x14:dxf>
               <font>
@@ -2639,8 +2744,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{A1E405FC-112F-4528-AA72-9DDD2F5A96B4}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{2AF17728-F7D1-4FC2-BEAD-2F7ACA18DEF8}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,F2)))</xm:f>
             <xm:f>Lookup!$E$3</xm:f>
             <x14:dxf>
               <font>
@@ -2653,8 +2758,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{10D4F4A8-549E-4809-94C0-FA303CB7E0A6}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{D0F3CF43-0EA3-452F-BF89-8DD10A003900}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,F2)))</xm:f>
             <xm:f>Lookup!$E$2</xm:f>
             <x14:dxf>
               <font>
@@ -2667,7 +2772,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E2:E100</xm:sqref>
+          <xm:sqref>F2:F100</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4064,7 +4169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC45D43-7DB0-4999-A671-8DD063ABA038}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixes #26 integrate conversion of PK Ratio plots (#56)
* Fixes #26 integrate conversion of PK Ratio plots

* Apply suggestions from code review

Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>

* Update template showing PK Ratio colors

---------

Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ACCB5F-0663-4CE0-B0B6-2E8E25C37A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0C9AF4-8E40-421B-9A36-129761BFCC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="1" activeTab="6" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="7" activeTab="14" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -873,7 +873,108 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="50">
+    <dxf>
+      <font>
+        <color rgb="FFCC6677"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC6677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF332288"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF332288"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDCC77"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDDCC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF117733"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF117733"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF88CCEE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF88CCEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF882255"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF882255"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF44AA99"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF44AA99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF999933"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAA4499"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA4499"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDDDDDD"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFCC6677"/>
@@ -2135,7 +2236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A769436E-1171-4487-BF5B-BA2851FAA4C1}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H100"/>
     </sheetView>
   </sheetViews>
@@ -2445,10 +2546,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A577CC0-D5A0-4A13-862C-A719AB883B03}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2456,12 +2557,13 @@
     <col min="1" max="1" width="25.81640625" customWidth="1"/>
     <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -2472,51 +2574,54 @@
         <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2526,8 +2631,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{122FD37C-2CD4-424F-8509-5E2E9FEA8569}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{4628622E-2F63-4491-A459-DB1F046D862C}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$11,F2)))</xm:f>
             <xm:f>Lookup!$E$11</xm:f>
             <x14:dxf>
               <font>
@@ -2540,8 +2645,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{62C66900-2092-418B-8DC2-8592CA91653C}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{E4A88C5B-61F3-48DF-9161-9DC4AD222169}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$10,F2)))</xm:f>
             <xm:f>Lookup!$E$10</xm:f>
             <x14:dxf>
               <font>
@@ -2554,8 +2659,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{E9D8C9E9-05BA-469B-8EB2-3B77645E7749}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{C753A7B6-EE29-4502-A4B3-4DB24EA9C6FA}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$9,F2)))</xm:f>
             <xm:f>Lookup!$E$9</xm:f>
             <x14:dxf>
               <font>
@@ -2568,8 +2673,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{BBD1427C-3DB1-48B0-BCD3-CE8B144AC0AD}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{A7363563-7105-4ED0-B895-D72413AB1510}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$8,F2)))</xm:f>
             <xm:f>Lookup!$E$8</xm:f>
             <x14:dxf>
               <font>
@@ -2582,8 +2687,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{C160719F-A188-4FE0-9C8C-74252EE20D95}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{20D19E1E-214A-4D14-BDB1-54F287803AD0}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$7,F2)))</xm:f>
             <xm:f>Lookup!$E$7</xm:f>
             <x14:dxf>
               <font>
@@ -2596,8 +2701,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{4A569E89-E3F0-42BA-95D8-4F9551719D1A}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{F4DC78DB-B917-4FE1-B2EC-5D205A6C99BB}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$6,F2)))</xm:f>
             <xm:f>Lookup!$E$6</xm:f>
             <x14:dxf>
               <font>
@@ -2610,8 +2715,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{8A00930E-F479-478A-8D4B-7E6C8B256E49}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{31946866-D629-4B7B-B3BA-E63CD387DA23}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$5,F2)))</xm:f>
             <xm:f>Lookup!$E$5</xm:f>
             <x14:dxf>
               <font>
@@ -2624,8 +2729,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{FD135833-5C75-4341-BD84-3B2F4162410A}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{DBEECD34-0320-470A-B068-24CFF47FC76E}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$4,F2)))</xm:f>
             <xm:f>Lookup!$E$4</xm:f>
             <x14:dxf>
               <font>
@@ -2639,8 +2744,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{A1E405FC-112F-4528-AA72-9DDD2F5A96B4}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{2AF17728-F7D1-4FC2-BEAD-2F7ACA18DEF8}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$3,F2)))</xm:f>
             <xm:f>Lookup!$E$3</xm:f>
             <x14:dxf>
               <font>
@@ -2653,8 +2758,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{10D4F4A8-549E-4809-94C0-FA303CB7E0A6}">
-            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,E2)))</xm:f>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{D0F3CF43-0EA3-452F-BF89-8DD10A003900}">
+            <xm:f>NOT(ISERROR(SEARCH(Lookup!$E$2,F2)))</xm:f>
             <xm:f>Lookup!$E$2</xm:f>
             <x14:dxf>
               <font>
@@ -2667,7 +2772,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E2:E100</xm:sqref>
+          <xm:sqref>F2:F100</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4064,7 +4169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC45D43-7DB0-4999-A671-8DD063ABA038}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixes #59 remove deprecated validation rule left in template
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0C9AF4-8E40-421B-9A36-129761BFCC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47089DA4-AC45-476D-991A-81AE46F240F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="7" activeTab="14" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-120" yWindow="-12120" windowWidth="19440" windowHeight="11520" tabRatio="814" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -873,108 +873,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <font>
-        <color rgb="FFCC6677"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC6677"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF332288"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF332288"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFDDCC77"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDDCC77"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF117733"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF117733"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF88CCEE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF88CCEE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF882255"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF882255"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF44AA99"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF44AA99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999933"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF999933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFAA4499"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAA4499"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFDDDDDD"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDDDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <font>
         <color rgb="FFCC6677"/>
@@ -2548,7 +2447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A577CC0-D5A0-4A13-862C-A719AB883B03}">
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F100"/>
     </sheetView>
   </sheetViews>
@@ -2914,7 +2813,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4031,7 +3932,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4054,18 +3955,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6DC1A308-6361-4F41-9EAC-41664F96AC49}">
-          <x14:formula1>
-            <xm:f>Projects!$A$2:$A$15</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixes #59 remove deprecated validation rule left in template (#73)
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0C9AF4-8E40-421B-9A36-129761BFCC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47089DA4-AC45-476D-991A-81AE46F240F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="7" activeTab="14" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-120" yWindow="-12120" windowWidth="19440" windowHeight="11520" tabRatio="814" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -873,108 +873,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <font>
-        <color rgb="FFCC6677"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC6677"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF332288"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF332288"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFDDCC77"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDDCC77"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF117733"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF117733"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF88CCEE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF88CCEE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF882255"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF882255"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF44AA99"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF44AA99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999933"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF999933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFAA4499"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAA4499"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFDDDDDD"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDDDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <font>
         <color rgb="FFCC6677"/>
@@ -2548,7 +2447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A577CC0-D5A0-4A13-862C-A719AB883B03}">
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F100"/>
     </sheetView>
   </sheetViews>
@@ -2914,7 +2813,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4031,7 +3932,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4054,18 +3955,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6DC1A308-6361-4F41-9EAC-41664F96AC49}">
-          <x14:formula1>
-            <xm:f>Projects!$A$2:$A$15</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixes #83 template header name matches updated header name
Template included a line break while created updated used a simple space
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47089DA4-AC45-476D-991A-81AE46F240F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCE3FB0-18C0-46A8-A75A-2B4E6AF53F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-12120" windowWidth="19440" windowHeight="11520" tabRatio="814" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="5385" yWindow="-12000" windowWidth="9810" windowHeight="11385" tabRatio="814" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -62,10 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="189">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="188">
   <si>
     <t>Path</t>
   </si>
@@ -103,9 +100,6 @@
     <t>DDIRatio</t>
   </si>
   <si>
-    <t>Observed Data</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -538,30 +532,6 @@
     <t>Simulation_Treatment</t>
   </si>
   <si>
-    <t>Control
-StartTime</t>
-  </si>
-  <si>
-    <t>Control
-EndTime</t>
-  </si>
-  <si>
-    <t>Control
-TimeUnit</t>
-  </si>
-  <si>
-    <t>Treatment
-StartTime</t>
-  </si>
-  <si>
-    <t>Treatment
-EndTime</t>
-  </si>
-  <si>
-    <t>Treatment
-TimeUnit</t>
-  </si>
-  <si>
     <t>Qualification plan schema version</t>
   </si>
   <si>
@@ -635,6 +605,27 @@
   </si>
   <si>
     <t>Concentration (molar)</t>
+  </si>
+  <si>
+    <t>ObservedData</t>
+  </si>
+  <si>
+    <t>Control StartTime</t>
+  </si>
+  <si>
+    <t>Control EndTime</t>
+  </si>
+  <si>
+    <t>Control TimeUnit</t>
+  </si>
+  <si>
+    <t>Treatment StartTime</t>
+  </si>
+  <si>
+    <t>Treatment EndTime</t>
+  </si>
+  <si>
+    <t>Treatment TimeUnit</t>
   </si>
 </sst>
 </file>
@@ -1624,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EDCB13-CEE1-4630-80E7-2767E804FDDB}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1635,12 +1626,12 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1652,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD237D21-BEEB-4E24-9FAD-AAF59B70B9A6}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H100"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1672,34 +1663,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1876,61 +1867,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="G1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="N1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1955,25 +1946,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2135,9 +2126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A769436E-1171-4487-BF5B-BA2851FAA4C1}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H100"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2149,70 +2138,70 @@
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="J1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="Q1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2374,8 +2363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432CE1B2-D2E2-4643-B063-1AD97C2500A1}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2396,46 +2385,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2447,9 +2436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A577CC0-D5A0-4A13-862C-A719AB883B03}">
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F100"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2464,64 +2451,64 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="O1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2695,25 +2682,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2737,16 +2724,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2766,7 +2753,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2779,7 +2766,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2792,16 +2779,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2813,9 +2800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2825,10 +2810,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2857,25 +2842,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2901,22 +2886,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2952,246 +2937,246 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="M1" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N1" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="P1" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="O2" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="9" t="b">
         <v>0</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="P3" s="9"/>
       <c r="Q3" s="9" t="b">
         <v>1</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>187</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="K4" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
       <c r="R4" s="9" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
@@ -3199,27 +3184,27 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
       <c r="R5" s="9" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -3227,7 +3212,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
@@ -3235,27 +3220,27 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="9" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -3263,7 +3248,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -3271,27 +3256,27 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="9" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -3299,7 +3284,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
@@ -3310,20 +3295,20 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -3331,7 +3316,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
@@ -3343,14 +3328,14 @@
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -3359,7 +3344,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
@@ -3373,10 +3358,10 @@
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -3385,7 +3370,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
@@ -3399,7 +3384,7 @@
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -3409,7 +3394,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
@@ -3423,7 +3408,7 @@
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -3433,7 +3418,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
@@ -3447,7 +3432,7 @@
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -3457,7 +3442,7 @@
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
@@ -3471,7 +3456,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -3481,7 +3466,7 @@
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
@@ -3495,7 +3480,7 @@
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -3505,7 +3490,7 @@
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
@@ -3519,7 +3504,7 @@
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -3529,7 +3514,7 @@
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
@@ -3543,7 +3528,7 @@
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -3553,7 +3538,7 @@
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
@@ -3567,7 +3552,7 @@
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -3577,7 +3562,7 @@
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
@@ -3591,7 +3576,7 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -3601,7 +3586,7 @@
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
@@ -3615,7 +3600,7 @@
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -3625,7 +3610,7 @@
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
@@ -3639,7 +3624,7 @@
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -3649,7 +3634,7 @@
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
@@ -3671,7 +3656,7 @@
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
@@ -3693,7 +3678,7 @@
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="L24" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
@@ -3715,7 +3700,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
       <c r="L25" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
@@ -3737,7 +3722,7 @@
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
@@ -3759,7 +3744,7 @@
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
@@ -3781,7 +3766,7 @@
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
@@ -3803,7 +3788,7 @@
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
@@ -3825,7 +3810,7 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
@@ -3847,7 +3832,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
@@ -3869,7 +3854,7 @@
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
@@ -3891,7 +3876,7 @@
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
       <c r="L33" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
@@ -3913,7 +3898,7 @@
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
@@ -3931,9 +3916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81057148-43A2-446A-9D02-6B1EAC2342A0}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3944,13 +3927,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3962,9 +3945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B84CD15-207B-431B-8E2A-C37D5F18D908}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3975,13 +3956,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3993,8 +3974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E91AF0-2BB9-4059-B6F7-322B449F2FE8}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4006,13 +3987,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4025,7 +4006,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4037,16 +4018,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4058,8 +4039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC45D43-7DB0-4999-A671-8DD063ABA038}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4073,19 +4054,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4098,7 +4079,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4109,13 +4090,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -4127,8 +4108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F83E462-CD2A-4A6E-B117-A1A1EAD04B68}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4151,55 +4132,55 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes #83 template header name matches updated header name (#85)
* Fixes #83 template header name matches updated header name

Template included a line break while created updated used a simple space

* Fix tests comparing headers
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47089DA4-AC45-476D-991A-81AE46F240F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCE3FB0-18C0-46A8-A75A-2B4E6AF53F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-12120" windowWidth="19440" windowHeight="11520" tabRatio="814" activeTab="1" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="5385" yWindow="-12000" windowWidth="9810" windowHeight="11385" tabRatio="814" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -62,10 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="189">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="188">
   <si>
     <t>Path</t>
   </si>
@@ -103,9 +100,6 @@
     <t>DDIRatio</t>
   </si>
   <si>
-    <t>Observed Data</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -538,30 +532,6 @@
     <t>Simulation_Treatment</t>
   </si>
   <si>
-    <t>Control
-StartTime</t>
-  </si>
-  <si>
-    <t>Control
-EndTime</t>
-  </si>
-  <si>
-    <t>Control
-TimeUnit</t>
-  </si>
-  <si>
-    <t>Treatment
-StartTime</t>
-  </si>
-  <si>
-    <t>Treatment
-EndTime</t>
-  </si>
-  <si>
-    <t>Treatment
-TimeUnit</t>
-  </si>
-  <si>
     <t>Qualification plan schema version</t>
   </si>
   <si>
@@ -635,6 +605,27 @@
   </si>
   <si>
     <t>Concentration (molar)</t>
+  </si>
+  <si>
+    <t>ObservedData</t>
+  </si>
+  <si>
+    <t>Control StartTime</t>
+  </si>
+  <si>
+    <t>Control EndTime</t>
+  </si>
+  <si>
+    <t>Control TimeUnit</t>
+  </si>
+  <si>
+    <t>Treatment StartTime</t>
+  </si>
+  <si>
+    <t>Treatment EndTime</t>
+  </si>
+  <si>
+    <t>Treatment TimeUnit</t>
   </si>
 </sst>
 </file>
@@ -1624,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EDCB13-CEE1-4630-80E7-2767E804FDDB}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1635,12 +1626,12 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1652,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD237D21-BEEB-4E24-9FAD-AAF59B70B9A6}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H100"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1672,34 +1663,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1876,61 +1867,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="G1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="N1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1955,25 +1946,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2135,9 +2126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A769436E-1171-4487-BF5B-BA2851FAA4C1}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H100"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2149,70 +2138,70 @@
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="J1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="Q1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2374,8 +2363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432CE1B2-D2E2-4643-B063-1AD97C2500A1}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2396,46 +2385,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2447,9 +2436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A577CC0-D5A0-4A13-862C-A719AB883B03}">
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F100"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2464,64 +2451,64 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="O1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2695,25 +2682,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2737,16 +2724,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2766,7 +2753,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2779,7 +2766,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2792,16 +2779,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2813,9 +2800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70E22B6-D36E-4BA4-A909-4DA2E1F994EE}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2825,10 +2810,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2857,25 +2842,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2901,22 +2886,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2952,246 +2937,246 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="M1" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N1" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="P1" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="O2" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="9" t="b">
         <v>0</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="P3" s="9"/>
       <c r="Q3" s="9" t="b">
         <v>1</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>187</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="K4" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
       <c r="R4" s="9" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
@@ -3199,27 +3184,27 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
       <c r="R5" s="9" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -3227,7 +3212,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
@@ -3235,27 +3220,27 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="9" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -3263,7 +3248,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -3271,27 +3256,27 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="9" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -3299,7 +3284,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
@@ -3310,20 +3295,20 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -3331,7 +3316,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
@@ -3343,14 +3328,14 @@
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -3359,7 +3344,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
@@ -3373,10 +3358,10 @@
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -3385,7 +3370,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
@@ -3399,7 +3384,7 @@
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -3409,7 +3394,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
@@ -3423,7 +3408,7 @@
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -3433,7 +3418,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
@@ -3447,7 +3432,7 @@
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -3457,7 +3442,7 @@
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
@@ -3471,7 +3456,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -3481,7 +3466,7 @@
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
@@ -3495,7 +3480,7 @@
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -3505,7 +3490,7 @@
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
@@ -3519,7 +3504,7 @@
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -3529,7 +3514,7 @@
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
@@ -3543,7 +3528,7 @@
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -3553,7 +3538,7 @@
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
@@ -3567,7 +3552,7 @@
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -3577,7 +3562,7 @@
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
@@ -3591,7 +3576,7 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -3601,7 +3586,7 @@
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
@@ -3615,7 +3600,7 @@
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -3625,7 +3610,7 @@
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
@@ -3639,7 +3624,7 @@
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -3649,7 +3634,7 @@
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
@@ -3671,7 +3656,7 @@
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
@@ -3693,7 +3678,7 @@
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="L24" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
@@ -3715,7 +3700,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
       <c r="L25" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
@@ -3737,7 +3722,7 @@
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
@@ -3759,7 +3744,7 @@
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
@@ -3781,7 +3766,7 @@
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
@@ -3803,7 +3788,7 @@
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
@@ -3825,7 +3810,7 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
@@ -3847,7 +3832,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
@@ -3869,7 +3854,7 @@
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
@@ -3891,7 +3876,7 @@
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
       <c r="L33" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
@@ -3913,7 +3898,7 @@
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
@@ -3931,9 +3916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81057148-43A2-446A-9D02-6B1EAC2342A0}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3944,13 +3927,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3962,9 +3945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B84CD15-207B-431B-8E2A-C37D5F18D908}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3975,13 +3956,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3993,8 +3974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E91AF0-2BB9-4059-B6F7-322B449F2FE8}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4006,13 +3987,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4025,7 +4006,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4037,16 +4018,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4058,8 +4039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC45D43-7DB0-4999-A671-8DD063ABA038}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4073,19 +4054,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4098,7 +4079,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4109,13 +4090,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -4127,8 +4108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F83E462-CD2A-4A6E-B117-A1A1EAD04B68}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4151,55 +4132,55 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorder PK Ratio Mapping columns in template to match data validation
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCE3FB0-18C0-46A8-A75A-2B4E6AF53F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75C111D-C454-4B71-A253-BFBD27D7F08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="-12000" windowWidth="9810" windowHeight="11385" tabRatio="814" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="9495" yWindow="-12000" windowWidth="9810" windowHeight="11385" tabRatio="814" firstSheet="12" activeTab="15" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -1615,7 +1615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EDCB13-CEE1-4630-80E7-2767E804FDDB}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2670,14 +2670,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5A9D53-FE8C-4361-AB33-ABCEC6AC2D66}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -2691,16 +2694,16 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
76 fill combinations (#95)
* Fixes #76 fill combinations not covered by qualification plan

* Reorder PK Ratio Mapping columns in template to match data validation

* Exclude inputs with no section reference
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCE3FB0-18C0-46A8-A75A-2B4E6AF53F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75C111D-C454-4B71-A253-BFBD27D7F08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="-12000" windowWidth="9810" windowHeight="11385" tabRatio="814" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="9495" yWindow="-12000" windowWidth="9810" windowHeight="11385" tabRatio="814" firstSheet="12" activeTab="15" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -1615,7 +1615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EDCB13-CEE1-4630-80E7-2767E804FDDB}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2670,14 +2670,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5A9D53-FE8C-4361-AB33-ABCEC6AC2D66}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -2691,16 +2694,16 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert incorrect fix and properly fix template column headers
Co-authored-by: Yuri05 <25061876+Yuri05@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -2090,27 +2090,27 @@
       </c>
       <c r="J1" s="8" t="inlineStr">
         <is>
+          <t>ArtifactsGOFPlots</t>
+        </is>
+      </c>
+      <c r="K1" s="8" t="inlineStr">
+        <is>
+          <t>subunitsDDIRatioPlots</t>
+        </is>
+      </c>
+      <c r="L1" s="8" t="inlineStr">
+        <is>
+          <t>PK Parameter</t>
+        </is>
+      </c>
+      <c r="M1" s="8" t="inlineStr">
+        <is>
+          <t>ObservedDataType</t>
+        </is>
+      </c>
+      <c r="N1" s="8" t="inlineStr">
+        <is>
           <t>GOFMergedPlotType</t>
-        </is>
-      </c>
-      <c r="K1" s="8" t="inlineStr">
-        <is>
-          <t>subunitsDDIRatioPlots</t>
-        </is>
-      </c>
-      <c r="L1" s="8" t="inlineStr">
-        <is>
-          <t>PK Parameter</t>
-        </is>
-      </c>
-      <c r="M1" s="8" t="inlineStr">
-        <is>
-          <t>ObservedDataType</t>
-        </is>
-      </c>
-      <c r="N1" s="8" t="inlineStr">
-        <is>
-          <t>ArtifactsGOFPlots</t>
         </is>
       </c>
       <c r="O1" s="8" t="inlineStr">

</xml_diff>

<commit_message>
Fixes #96 swap Artifacts and Plot Type column in Excel template
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75C111D-C454-4B71-A253-BFBD27D7F08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C0C0C7-A9BA-4E71-8ED3-CA0814D5530F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="-12000" windowWidth="9810" windowHeight="11385" tabRatio="814" firstSheet="12" activeTab="15" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="10" activeTab="10" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -1853,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3301F9-9944-4A4A-8E79-17917B82ED2F}">
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1873,10 +1873,10 @@
         <v>14</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>38</v>
@@ -2670,7 +2670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5A9D53-FE8C-4361-AB33-ABCEC6AC2D66}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixes #96 swap Artifacts and Plot Type column in Excel template (#101)
</commit_message>
<xml_diff>
--- a/inst/Qualification-Template.xlsx
+++ b/inst/Qualification-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.QualificationPlanEditor\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75C111D-C454-4B71-A253-BFBD27D7F08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C0C0C7-A9BA-4E71-8ED3-CA0814D5530F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="-12000" windowWidth="9810" windowHeight="11385" tabRatio="814" firstSheet="12" activeTab="15" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="814" firstSheet="10" activeTab="10" xr2:uid="{784D6A16-FFDD-4362-8C3A-230B51BBD216}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaInfo" sheetId="16" r:id="rId1"/>
@@ -1853,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3301F9-9944-4A4A-8E79-17917B82ED2F}">
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1873,10 +1873,10 @@
         <v>14</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>38</v>
@@ -2670,7 +2670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5A9D53-FE8C-4361-AB33-ABCEC6AC2D66}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>